<commit_message>
Restructures directory and updates from current week to files
</commit_message>
<xml_diff>
--- a/Release_Candidate_3/t_toolbox_Release_Comparison.xlsx
+++ b/Release_Candidate_3/t_toolbox_Release_Comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2016\Programming\R-Project\r_toolbox\Release_Candidate_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2017\Programming\R-Project\r_toolbox\Release_Candidate_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>Module</t>
   </si>
@@ -68,9 +68,6 @@
     <t>t_definitions</t>
   </si>
   <si>
-    <t>t_find_originals_and_duplicates</t>
-  </si>
-  <si>
     <t>t_get_factor_levels</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>changed</t>
+  </si>
+  <si>
+    <t>t_delete_empty_variales</t>
   </si>
 </sst>
 </file>
@@ -428,25 +428,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -471,10 +471,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -488,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -499,10 +499,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -530,51 +530,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -586,9 +584,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -600,9 +598,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -614,115 +612,129 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>